<commit_message>
Add docs and e2e test
</commit_message>
<xml_diff>
--- a/src/test/resources/test-event-logs.xlsx
+++ b/src/test/resources/test-event-logs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/i530753/Desktop/University/VVPS/vvps-project/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF096986-3443-684A-949E-769830ADE56A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CE87E0B-B59E-C34E-AA08-DE12439406E8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="29020" windowHeight="14000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -892,7 +892,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>